<commit_message>
RP2 2016 Q2 data release
</commit_message>
<xml_diff>
--- a/data/2016/RP2 - CIV_MIL_2016.xlsx
+++ b/data/2016/RP2 - CIV_MIL_2016.xlsx
@@ -29,13 +29,13 @@
     <t>EUROCONTROL - PRB</t>
   </si>
   <si>
+    <t>Period Start</t>
+  </si>
+  <si>
     <t>Period</t>
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>Period Start</t>
   </si>
   <si>
     <t>Meta data</t>
@@ -218,14 +218,14 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color rgb="FFC00000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="10"/>
@@ -323,24 +323,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -353,23 +350,26 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -713,11 +713,11 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>6</v>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="D1" s="7">
         <v>42005</v>
@@ -725,40 +725,40 @@
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="29">
         <v>42436</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2" s="12">
         <v>42369</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -768,8 +768,8 @@
         <v>365</v>
       </c>
       <c r="D4" s="21"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
@@ -782,8 +782,8 @@
         <v>17</v>
       </c>
       <c r="D5" s="24"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
@@ -796,8 +796,8 @@
         <v>1035</v>
       </c>
       <c r="D6" s="27"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
@@ -806,8 +806,8 @@
       <c r="B7" s="27"/>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
@@ -816,8 +816,8 @@
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
@@ -828,8 +828,8 @@
       <c r="D9" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
@@ -838,8 +838,8 @@
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
@@ -852,8 +852,8 @@
         <v>42029</v>
       </c>
       <c r="D11" s="27"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
@@ -866,8 +866,8 @@
         <v>2525</v>
       </c>
       <c r="D12" s="27"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
@@ -880,8 +880,8 @@
         <v>2289</v>
       </c>
       <c r="D13" s="27"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
     </row>
     <row r="14" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
@@ -890,8 +890,8 @@
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
@@ -904,8 +904,8 @@
         <v>13033</v>
       </c>
       <c r="D15" s="27"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
@@ -918,8 +918,8 @@
         <v>35272</v>
       </c>
       <c r="D16" s="27"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
@@ -928,8 +928,8 @@
       <c r="B17" s="27"/>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
     </row>
     <row r="18" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
@@ -938,8 +938,8 @@
       <c r="B18" s="27"/>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
@@ -950,8 +950,8 @@
       <c r="D19" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
@@ -964,8 +964,8 @@
         <v>3322</v>
       </c>
       <c r="D20" s="27"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
     </row>
     <row r="21" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
@@ -978,8 +978,8 @@
         <v>921</v>
       </c>
       <c r="D21" s="27"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
     </row>
     <row r="22" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
@@ -992,8 +992,8 @@
         <v>12143</v>
       </c>
       <c r="D22" s="27"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
     </row>
     <row r="23" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
@@ -1004,8 +1004,8 @@
       <c r="D23" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
     </row>
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
@@ -1016,8 +1016,8 @@
       <c r="D24" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
@@ -1028,8 +1028,8 @@
       <c r="D25" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
@@ -1042,8 +1042,8 @@
         <v>14422</v>
       </c>
       <c r="D26" s="27"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
     </row>
     <row r="27" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
@@ -1056,8 +1056,8 @@
         <v>3212</v>
       </c>
       <c r="D27" s="27"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="25" t="s">
@@ -1070,8 +1070,8 @@
         <v>95580</v>
       </c>
       <c r="D28" s="27"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
     </row>
     <row r="29" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="25" t="s">
@@ -1082,8 +1082,8 @@
       <c r="D29" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
     </row>
     <row r="30" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
@@ -1096,8 +1096,8 @@
         <v>49928</v>
       </c>
       <c r="D30" s="27"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="31" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
@@ -1110,8 +1110,8 @@
         <v>68784</v>
       </c>
       <c r="D31" s="27"/>
-      <c r="E31" s="18"/>
-      <c r="F31" s="18"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
     </row>
     <row r="32" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
@@ -1120,8 +1120,8 @@
       <c r="B32" s="27"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
     </row>
     <row r="33" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
@@ -1134,8 +1134,8 @@
         <v>6922</v>
       </c>
       <c r="D33" s="27"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
     </row>
     <row r="34" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
@@ -1148,8 +1148,8 @@
         <v>377</v>
       </c>
       <c r="D34" s="27"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
@@ -1158,8 +1158,8 @@
       <c r="B35" s="27"/>
       <c r="C35" s="27"/>
       <c r="D35" s="27"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
     </row>
     <row r="36" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
@@ -1172,8 +1172,8 @@
         <v>24676</v>
       </c>
       <c r="D36" s="27"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1198,81 +1198,81 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="15"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="15"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="15"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>

</xml_diff>